<commit_message>
fix: adding school and education for scholar bulk upload
</commit_message>
<xml_diff>
--- a/frontend/src/components/components/Donor Application Multiple.xlsx
+++ b/frontend/src/components/components/Donor Application Multiple.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>Last Name *</t>
   </si>
@@ -60,13 +60,19 @@
     <t>Years Involved *</t>
   </si>
   <si>
-    <t>Other Details *</t>
-  </si>
-  <si>
     <t>Donor</t>
   </si>
   <si>
     <t>Reason/s for Applying</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Details *</t>
   </si>
 </sst>
 </file>
@@ -98,7 +104,7 @@
       <name val="Corbel"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -115,6 +121,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFEF2"/>
         <bgColor rgb="FFFFFEF2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor rgb="FFFFFEF2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -227,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -250,6 +268,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,89 +493,130 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q160"/>
+  <dimension ref="A1:S161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="17" width="21.36328125" customWidth="1"/>
+    <col min="1" max="11" width="21.36328125" customWidth="1"/>
+    <col min="12" max="12" width="0.90625" style="10" customWidth="1"/>
+    <col min="13" max="19" width="21.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="8"/>
+      <c r="M1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="2"/>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -562,14 +628,16 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="L3" s="9"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="1"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -581,14 +649,16 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="L4" s="9"/>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -600,14 +670,16 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="L5" s="9"/>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
-      <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -619,14 +691,16 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="L6" s="9"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="1"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -638,14 +712,16 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="L7" s="9"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
-      <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -657,14 +733,16 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="L8" s="9"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
-      <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -676,14 +754,16 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="L9" s="9"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -695,14 +775,16 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="L10" s="9"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-      <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="1"/>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -714,14 +796,16 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="L11" s="9"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-      <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="1"/>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -733,14 +817,16 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="L12" s="9"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
-      <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="1"/>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -752,14 +838,16 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="L13" s="9"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
-      <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="1"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -771,14 +859,16 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="L14" s="9"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
-      <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="1"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -790,14 +880,16 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="L15" s="9"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="1"/>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -809,14 +901,16 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="L16" s="9"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
-      <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="1"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -828,14 +922,16 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="L17" s="9"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
-      <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="1"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -847,14 +943,16 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="L18" s="9"/>
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
-      <c r="Q18" s="1"/>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="1"/>
+    </row>
+    <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -866,14 +964,16 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="L19" s="9"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
-      <c r="Q19" s="1"/>
-    </row>
-    <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="1"/>
+    </row>
+    <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -885,14 +985,16 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
-      <c r="L20" s="3"/>
+      <c r="L20" s="9"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
-      <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="1"/>
+    </row>
+    <row r="21" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -904,14 +1006,16 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
-      <c r="L21" s="3"/>
+      <c r="L21" s="9"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
-      <c r="Q21" s="1"/>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -923,14 +1027,16 @@
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
-      <c r="L22" s="3"/>
+      <c r="L22" s="9"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
-      <c r="Q22" s="1"/>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="1"/>
+    </row>
+    <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -942,14 +1048,16 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="L23" s="9"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
-      <c r="Q23" s="1"/>
-    </row>
-    <row r="24" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="1"/>
+    </row>
+    <row r="24" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -961,14 +1069,16 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
+      <c r="L24" s="9"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
-      <c r="Q24" s="1"/>
-    </row>
-    <row r="25" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="1"/>
+    </row>
+    <row r="25" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -980,14 +1090,16 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+      <c r="L25" s="9"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
-      <c r="Q25" s="1"/>
-    </row>
-    <row r="26" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="1"/>
+    </row>
+    <row r="26" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -999,14 +1111,16 @@
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
+      <c r="L26" s="9"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
-      <c r="Q26" s="1"/>
-    </row>
-    <row r="27" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="1"/>
+    </row>
+    <row r="27" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1018,14 +1132,16 @@
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-      <c r="L27" s="3"/>
+      <c r="L27" s="9"/>
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
-      <c r="Q27" s="1"/>
-    </row>
-    <row r="28" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="1"/>
+    </row>
+    <row r="28" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1037,14 +1153,16 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
+      <c r="L28" s="9"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
-      <c r="Q28" s="1"/>
-    </row>
-    <row r="29" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="1"/>
+    </row>
+    <row r="29" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1056,14 +1174,16 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
-      <c r="L29" s="3"/>
+      <c r="L29" s="9"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
-      <c r="Q29" s="1"/>
-    </row>
-    <row r="30" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="1"/>
+    </row>
+    <row r="30" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1075,14 +1195,16 @@
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
+      <c r="L30" s="9"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
-      <c r="Q30" s="1"/>
-    </row>
-    <row r="31" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="1"/>
+    </row>
+    <row r="31" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1094,14 +1216,16 @@
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
+      <c r="L31" s="9"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
-      <c r="Q31" s="1"/>
-    </row>
-    <row r="32" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="1"/>
+    </row>
+    <row r="32" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1113,14 +1237,16 @@
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
+      <c r="L32" s="9"/>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
-      <c r="Q32" s="1"/>
-    </row>
-    <row r="33" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="1"/>
+    </row>
+    <row r="33" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1132,14 +1258,16 @@
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
+      <c r="L33" s="9"/>
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
-      <c r="Q33" s="1"/>
-    </row>
-    <row r="34" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="1"/>
+    </row>
+    <row r="34" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -1151,14 +1279,16 @@
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
+      <c r="L34" s="9"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
-      <c r="Q34" s="1"/>
-    </row>
-    <row r="35" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="1"/>
+    </row>
+    <row r="35" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -1170,14 +1300,16 @@
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
+      <c r="L35" s="9"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
-      <c r="Q35" s="1"/>
-    </row>
-    <row r="36" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="1"/>
+    </row>
+    <row r="36" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1189,14 +1321,16 @@
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
+      <c r="L36" s="9"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
-      <c r="Q36" s="1"/>
-    </row>
-    <row r="37" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="1"/>
+    </row>
+    <row r="37" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -1208,14 +1342,16 @@
       <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
+      <c r="L37" s="9"/>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
-      <c r="Q37" s="1"/>
-    </row>
-    <row r="38" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="1"/>
+    </row>
+    <row r="38" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -1227,14 +1363,16 @@
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
+      <c r="L38" s="9"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
-      <c r="Q38" s="1"/>
-    </row>
-    <row r="39" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="1"/>
+    </row>
+    <row r="39" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1246,14 +1384,16 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
+      <c r="L39" s="9"/>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
-      <c r="Q39" s="1"/>
-    </row>
-    <row r="40" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="1"/>
+    </row>
+    <row r="40" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -1265,14 +1405,16 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
+      <c r="L40" s="9"/>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
-      <c r="Q40" s="1"/>
-    </row>
-    <row r="41" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="1"/>
+    </row>
+    <row r="41" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -1284,14 +1426,16 @@
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
+      <c r="L41" s="9"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
-      <c r="Q41" s="1"/>
-    </row>
-    <row r="42" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="1"/>
+    </row>
+    <row r="42" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -1303,14 +1447,16 @@
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
+      <c r="L42" s="9"/>
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
       <c r="P42" s="3"/>
-      <c r="Q42" s="1"/>
-    </row>
-    <row r="43" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="1"/>
+    </row>
+    <row r="43" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -1322,14 +1468,16 @@
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
+      <c r="L43" s="9"/>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
-      <c r="Q43" s="1"/>
-    </row>
-    <row r="44" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="1"/>
+    </row>
+    <row r="44" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1341,14 +1489,16 @@
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
+      <c r="L44" s="9"/>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
-      <c r="Q44" s="1"/>
-    </row>
-    <row r="45" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="1"/>
+    </row>
+    <row r="45" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1360,14 +1510,16 @@
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
+      <c r="L45" s="9"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
-      <c r="Q45" s="1"/>
-    </row>
-    <row r="46" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="1"/>
+    </row>
+    <row r="46" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1379,14 +1531,16 @@
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
+      <c r="L46" s="9"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
-      <c r="Q46" s="1"/>
-    </row>
-    <row r="47" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="1"/>
+    </row>
+    <row r="47" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -1398,14 +1552,16 @@
       <c r="I47" s="3"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
+      <c r="L47" s="9"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
-      <c r="Q47" s="1"/>
-    </row>
-    <row r="48" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="1"/>
+    </row>
+    <row r="48" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -1417,14 +1573,16 @@
       <c r="I48" s="3"/>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
+      <c r="L48" s="9"/>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
-      <c r="Q48" s="1"/>
-    </row>
-    <row r="49" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="1"/>
+    </row>
+    <row r="49" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -1436,14 +1594,16 @@
       <c r="I49" s="3"/>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
+      <c r="L49" s="9"/>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
       <c r="P49" s="3"/>
-      <c r="Q49" s="1"/>
-    </row>
-    <row r="50" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="1"/>
+    </row>
+    <row r="50" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1455,14 +1615,16 @@
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
+      <c r="L50" s="9"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
-      <c r="Q50" s="1"/>
-    </row>
-    <row r="51" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="1"/>
+    </row>
+    <row r="51" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -1474,14 +1636,16 @@
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
+      <c r="L51" s="9"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
-      <c r="Q51" s="1"/>
-    </row>
-    <row r="52" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="1"/>
+    </row>
+    <row r="52" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -1493,14 +1657,16 @@
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
+      <c r="L52" s="9"/>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
-      <c r="Q52" s="1"/>
-    </row>
-    <row r="53" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="1"/>
+    </row>
+    <row r="53" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -1512,14 +1678,16 @@
       <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
+      <c r="L53" s="9"/>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
       <c r="P53" s="3"/>
-      <c r="Q53" s="1"/>
-    </row>
-    <row r="54" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="1"/>
+    </row>
+    <row r="54" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -1531,14 +1699,16 @@
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
-      <c r="L54" s="3"/>
+      <c r="L54" s="9"/>
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
       <c r="P54" s="3"/>
-      <c r="Q54" s="1"/>
-    </row>
-    <row r="55" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q54" s="3"/>
+      <c r="R54" s="3"/>
+      <c r="S54" s="1"/>
+    </row>
+    <row r="55" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -1550,14 +1720,16 @@
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
+      <c r="L55" s="9"/>
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
       <c r="O55" s="3"/>
       <c r="P55" s="3"/>
-      <c r="Q55" s="1"/>
-    </row>
-    <row r="56" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="1"/>
+    </row>
+    <row r="56" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -1569,14 +1741,16 @@
       <c r="I56" s="3"/>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
+      <c r="L56" s="9"/>
       <c r="M56" s="3"/>
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
       <c r="P56" s="3"/>
-      <c r="Q56" s="1"/>
-    </row>
-    <row r="57" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="1"/>
+    </row>
+    <row r="57" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -1588,14 +1762,16 @@
       <c r="I57" s="3"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
-      <c r="L57" s="3"/>
+      <c r="L57" s="9"/>
       <c r="M57" s="3"/>
       <c r="N57" s="3"/>
       <c r="O57" s="3"/>
       <c r="P57" s="3"/>
-      <c r="Q57" s="1"/>
-    </row>
-    <row r="58" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="1"/>
+    </row>
+    <row r="58" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -1607,14 +1783,16 @@
       <c r="I58" s="3"/>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
+      <c r="L58" s="9"/>
       <c r="M58" s="3"/>
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
       <c r="P58" s="3"/>
-      <c r="Q58" s="1"/>
-    </row>
-    <row r="59" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="1"/>
+    </row>
+    <row r="59" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -1626,14 +1804,16 @@
       <c r="I59" s="3"/>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
-      <c r="L59" s="3"/>
+      <c r="L59" s="9"/>
       <c r="M59" s="3"/>
       <c r="N59" s="3"/>
       <c r="O59" s="3"/>
       <c r="P59" s="3"/>
-      <c r="Q59" s="1"/>
-    </row>
-    <row r="60" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="1"/>
+    </row>
+    <row r="60" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -1645,14 +1825,16 @@
       <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
-      <c r="L60" s="3"/>
+      <c r="L60" s="9"/>
       <c r="M60" s="3"/>
       <c r="N60" s="3"/>
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
-      <c r="Q60" s="1"/>
-    </row>
-    <row r="61" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="1"/>
+    </row>
+    <row r="61" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -1664,14 +1846,16 @@
       <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
+      <c r="L61" s="9"/>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>
       <c r="O61" s="3"/>
       <c r="P61" s="3"/>
-      <c r="Q61" s="1"/>
-    </row>
-    <row r="62" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q61" s="3"/>
+      <c r="R61" s="3"/>
+      <c r="S61" s="1"/>
+    </row>
+    <row r="62" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -1683,14 +1867,16 @@
       <c r="I62" s="3"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
-      <c r="L62" s="3"/>
+      <c r="L62" s="9"/>
       <c r="M62" s="3"/>
       <c r="N62" s="3"/>
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
-      <c r="Q62" s="1"/>
-    </row>
-    <row r="63" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="1"/>
+    </row>
+    <row r="63" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -1702,14 +1888,16 @@
       <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
-      <c r="L63" s="3"/>
+      <c r="L63" s="9"/>
       <c r="M63" s="3"/>
       <c r="N63" s="3"/>
       <c r="O63" s="3"/>
       <c r="P63" s="3"/>
-      <c r="Q63" s="1"/>
-    </row>
-    <row r="64" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="1"/>
+    </row>
+    <row r="64" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -1721,14 +1909,16 @@
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
-      <c r="L64" s="3"/>
+      <c r="L64" s="9"/>
       <c r="M64" s="3"/>
       <c r="N64" s="3"/>
       <c r="O64" s="3"/>
       <c r="P64" s="3"/>
-      <c r="Q64" s="1"/>
-    </row>
-    <row r="65" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q64" s="3"/>
+      <c r="R64" s="3"/>
+      <c r="S64" s="1"/>
+    </row>
+    <row r="65" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -1740,14 +1930,16 @@
       <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
-      <c r="L65" s="3"/>
+      <c r="L65" s="9"/>
       <c r="M65" s="3"/>
       <c r="N65" s="3"/>
       <c r="O65" s="3"/>
       <c r="P65" s="3"/>
-      <c r="Q65" s="1"/>
-    </row>
-    <row r="66" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="1"/>
+    </row>
+    <row r="66" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -1759,14 +1951,16 @@
       <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
-      <c r="L66" s="3"/>
+      <c r="L66" s="9"/>
       <c r="M66" s="3"/>
       <c r="N66" s="3"/>
       <c r="O66" s="3"/>
       <c r="P66" s="3"/>
-      <c r="Q66" s="1"/>
-    </row>
-    <row r="67" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q66" s="3"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="1"/>
+    </row>
+    <row r="67" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -1778,14 +1972,16 @@
       <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
-      <c r="L67" s="3"/>
+      <c r="L67" s="9"/>
       <c r="M67" s="3"/>
       <c r="N67" s="3"/>
       <c r="O67" s="3"/>
       <c r="P67" s="3"/>
-      <c r="Q67" s="1"/>
-    </row>
-    <row r="68" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="1"/>
+    </row>
+    <row r="68" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -1797,14 +1993,16 @@
       <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
-      <c r="L68" s="3"/>
+      <c r="L68" s="9"/>
       <c r="M68" s="3"/>
       <c r="N68" s="3"/>
       <c r="O68" s="3"/>
       <c r="P68" s="3"/>
-      <c r="Q68" s="1"/>
-    </row>
-    <row r="69" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="1"/>
+    </row>
+    <row r="69" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -1816,14 +2014,16 @@
       <c r="I69" s="3"/>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
-      <c r="L69" s="3"/>
+      <c r="L69" s="9"/>
       <c r="M69" s="3"/>
       <c r="N69" s="3"/>
       <c r="O69" s="3"/>
       <c r="P69" s="3"/>
-      <c r="Q69" s="1"/>
-    </row>
-    <row r="70" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q69" s="3"/>
+      <c r="R69" s="3"/>
+      <c r="S69" s="1"/>
+    </row>
+    <row r="70" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -1835,14 +2035,16 @@
       <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
-      <c r="L70" s="3"/>
+      <c r="L70" s="9"/>
       <c r="M70" s="3"/>
       <c r="N70" s="3"/>
       <c r="O70" s="3"/>
       <c r="P70" s="3"/>
-      <c r="Q70" s="1"/>
-    </row>
-    <row r="71" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="1"/>
+    </row>
+    <row r="71" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -1854,14 +2056,16 @@
       <c r="I71" s="3"/>
       <c r="J71" s="3"/>
       <c r="K71" s="3"/>
-      <c r="L71" s="3"/>
+      <c r="L71" s="9"/>
       <c r="M71" s="3"/>
       <c r="N71" s="3"/>
       <c r="O71" s="3"/>
       <c r="P71" s="3"/>
-      <c r="Q71" s="1"/>
-    </row>
-    <row r="72" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="1"/>
+    </row>
+    <row r="72" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -1873,14 +2077,16 @@
       <c r="I72" s="3"/>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
-      <c r="L72" s="3"/>
+      <c r="L72" s="9"/>
       <c r="M72" s="3"/>
       <c r="N72" s="3"/>
       <c r="O72" s="3"/>
       <c r="P72" s="3"/>
-      <c r="Q72" s="1"/>
-    </row>
-    <row r="73" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q72" s="3"/>
+      <c r="R72" s="3"/>
+      <c r="S72" s="1"/>
+    </row>
+    <row r="73" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -1892,14 +2098,16 @@
       <c r="I73" s="3"/>
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
-      <c r="L73" s="3"/>
+      <c r="L73" s="9"/>
       <c r="M73" s="3"/>
       <c r="N73" s="3"/>
       <c r="O73" s="3"/>
       <c r="P73" s="3"/>
-      <c r="Q73" s="1"/>
-    </row>
-    <row r="74" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q73" s="3"/>
+      <c r="R73" s="3"/>
+      <c r="S73" s="1"/>
+    </row>
+    <row r="74" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -1911,14 +2119,16 @@
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
-      <c r="L74" s="3"/>
+      <c r="L74" s="9"/>
       <c r="M74" s="3"/>
       <c r="N74" s="3"/>
       <c r="O74" s="3"/>
       <c r="P74" s="3"/>
-      <c r="Q74" s="1"/>
-    </row>
-    <row r="75" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q74" s="3"/>
+      <c r="R74" s="3"/>
+      <c r="S74" s="1"/>
+    </row>
+    <row r="75" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -1930,14 +2140,16 @@
       <c r="I75" s="3"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
-      <c r="L75" s="3"/>
+      <c r="L75" s="9"/>
       <c r="M75" s="3"/>
       <c r="N75" s="3"/>
       <c r="O75" s="3"/>
       <c r="P75" s="3"/>
-      <c r="Q75" s="1"/>
-    </row>
-    <row r="76" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q75" s="3"/>
+      <c r="R75" s="3"/>
+      <c r="S75" s="1"/>
+    </row>
+    <row r="76" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -1949,14 +2161,16 @@
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
-      <c r="L76" s="3"/>
+      <c r="L76" s="9"/>
       <c r="M76" s="3"/>
       <c r="N76" s="3"/>
       <c r="O76" s="3"/>
       <c r="P76" s="3"/>
-      <c r="Q76" s="1"/>
-    </row>
-    <row r="77" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q76" s="3"/>
+      <c r="R76" s="3"/>
+      <c r="S76" s="1"/>
+    </row>
+    <row r="77" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -1968,14 +2182,16 @@
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
       <c r="K77" s="3"/>
-      <c r="L77" s="3"/>
+      <c r="L77" s="9"/>
       <c r="M77" s="3"/>
       <c r="N77" s="3"/>
       <c r="O77" s="3"/>
       <c r="P77" s="3"/>
-      <c r="Q77" s="1"/>
-    </row>
-    <row r="78" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q77" s="3"/>
+      <c r="R77" s="3"/>
+      <c r="S77" s="1"/>
+    </row>
+    <row r="78" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -1987,14 +2203,16 @@
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
       <c r="K78" s="3"/>
-      <c r="L78" s="3"/>
+      <c r="L78" s="9"/>
       <c r="M78" s="3"/>
       <c r="N78" s="3"/>
       <c r="O78" s="3"/>
       <c r="P78" s="3"/>
-      <c r="Q78" s="1"/>
-    </row>
-    <row r="79" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q78" s="3"/>
+      <c r="R78" s="3"/>
+      <c r="S78" s="1"/>
+    </row>
+    <row r="79" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -2006,14 +2224,16 @@
       <c r="I79" s="3"/>
       <c r="J79" s="3"/>
       <c r="K79" s="3"/>
-      <c r="L79" s="3"/>
+      <c r="L79" s="9"/>
       <c r="M79" s="3"/>
       <c r="N79" s="3"/>
       <c r="O79" s="3"/>
       <c r="P79" s="3"/>
-      <c r="Q79" s="1"/>
-    </row>
-    <row r="80" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q79" s="3"/>
+      <c r="R79" s="3"/>
+      <c r="S79" s="1"/>
+    </row>
+    <row r="80" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -2025,14 +2245,16 @@
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
       <c r="K80" s="3"/>
-      <c r="L80" s="3"/>
+      <c r="L80" s="9"/>
       <c r="M80" s="3"/>
       <c r="N80" s="3"/>
       <c r="O80" s="3"/>
       <c r="P80" s="3"/>
-      <c r="Q80" s="1"/>
-    </row>
-    <row r="81" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q80" s="3"/>
+      <c r="R80" s="3"/>
+      <c r="S80" s="1"/>
+    </row>
+    <row r="81" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -2044,14 +2266,16 @@
       <c r="I81" s="3"/>
       <c r="J81" s="3"/>
       <c r="K81" s="3"/>
-      <c r="L81" s="3"/>
+      <c r="L81" s="9"/>
       <c r="M81" s="3"/>
       <c r="N81" s="3"/>
       <c r="O81" s="3"/>
       <c r="P81" s="3"/>
-      <c r="Q81" s="1"/>
-    </row>
-    <row r="82" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q81" s="3"/>
+      <c r="R81" s="3"/>
+      <c r="S81" s="1"/>
+    </row>
+    <row r="82" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -2063,14 +2287,16 @@
       <c r="I82" s="3"/>
       <c r="J82" s="3"/>
       <c r="K82" s="3"/>
-      <c r="L82" s="3"/>
+      <c r="L82" s="9"/>
       <c r="M82" s="3"/>
       <c r="N82" s="3"/>
       <c r="O82" s="3"/>
       <c r="P82" s="3"/>
-      <c r="Q82" s="1"/>
-    </row>
-    <row r="83" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q82" s="3"/>
+      <c r="R82" s="3"/>
+      <c r="S82" s="1"/>
+    </row>
+    <row r="83" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -2082,14 +2308,16 @@
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
       <c r="K83" s="3"/>
-      <c r="L83" s="3"/>
+      <c r="L83" s="9"/>
       <c r="M83" s="3"/>
       <c r="N83" s="3"/>
       <c r="O83" s="3"/>
       <c r="P83" s="3"/>
-      <c r="Q83" s="1"/>
-    </row>
-    <row r="84" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q83" s="3"/>
+      <c r="R83" s="3"/>
+      <c r="S83" s="1"/>
+    </row>
+    <row r="84" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -2101,14 +2329,16 @@
       <c r="I84" s="3"/>
       <c r="J84" s="3"/>
       <c r="K84" s="3"/>
-      <c r="L84" s="3"/>
+      <c r="L84" s="9"/>
       <c r="M84" s="3"/>
       <c r="N84" s="3"/>
       <c r="O84" s="3"/>
       <c r="P84" s="3"/>
-      <c r="Q84" s="1"/>
-    </row>
-    <row r="85" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q84" s="3"/>
+      <c r="R84" s="3"/>
+      <c r="S84" s="1"/>
+    </row>
+    <row r="85" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -2120,14 +2350,16 @@
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3"/>
-      <c r="L85" s="3"/>
+      <c r="L85" s="9"/>
       <c r="M85" s="3"/>
       <c r="N85" s="3"/>
       <c r="O85" s="3"/>
       <c r="P85" s="3"/>
-      <c r="Q85" s="1"/>
-    </row>
-    <row r="86" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q85" s="3"/>
+      <c r="R85" s="3"/>
+      <c r="S85" s="1"/>
+    </row>
+    <row r="86" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -2139,14 +2371,16 @@
       <c r="I86" s="3"/>
       <c r="J86" s="3"/>
       <c r="K86" s="3"/>
-      <c r="L86" s="3"/>
+      <c r="L86" s="9"/>
       <c r="M86" s="3"/>
       <c r="N86" s="3"/>
       <c r="O86" s="3"/>
       <c r="P86" s="3"/>
-      <c r="Q86" s="1"/>
-    </row>
-    <row r="87" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q86" s="3"/>
+      <c r="R86" s="3"/>
+      <c r="S86" s="1"/>
+    </row>
+    <row r="87" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -2158,14 +2392,16 @@
       <c r="I87" s="3"/>
       <c r="J87" s="3"/>
       <c r="K87" s="3"/>
-      <c r="L87" s="3"/>
+      <c r="L87" s="9"/>
       <c r="M87" s="3"/>
       <c r="N87" s="3"/>
       <c r="O87" s="3"/>
       <c r="P87" s="3"/>
-      <c r="Q87" s="1"/>
-    </row>
-    <row r="88" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q87" s="3"/>
+      <c r="R87" s="3"/>
+      <c r="S87" s="1"/>
+    </row>
+    <row r="88" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -2177,14 +2413,16 @@
       <c r="I88" s="3"/>
       <c r="J88" s="3"/>
       <c r="K88" s="3"/>
-      <c r="L88" s="3"/>
+      <c r="L88" s="9"/>
       <c r="M88" s="3"/>
       <c r="N88" s="3"/>
       <c r="O88" s="3"/>
       <c r="P88" s="3"/>
-      <c r="Q88" s="1"/>
-    </row>
-    <row r="89" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q88" s="3"/>
+      <c r="R88" s="3"/>
+      <c r="S88" s="1"/>
+    </row>
+    <row r="89" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -2196,14 +2434,16 @@
       <c r="I89" s="3"/>
       <c r="J89" s="3"/>
       <c r="K89" s="3"/>
-      <c r="L89" s="3"/>
+      <c r="L89" s="9"/>
       <c r="M89" s="3"/>
       <c r="N89" s="3"/>
       <c r="O89" s="3"/>
       <c r="P89" s="3"/>
-      <c r="Q89" s="1"/>
-    </row>
-    <row r="90" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q89" s="3"/>
+      <c r="R89" s="3"/>
+      <c r="S89" s="1"/>
+    </row>
+    <row r="90" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -2215,14 +2455,16 @@
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
       <c r="K90" s="3"/>
-      <c r="L90" s="3"/>
+      <c r="L90" s="9"/>
       <c r="M90" s="3"/>
       <c r="N90" s="3"/>
       <c r="O90" s="3"/>
       <c r="P90" s="3"/>
-      <c r="Q90" s="1"/>
-    </row>
-    <row r="91" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q90" s="3"/>
+      <c r="R90" s="3"/>
+      <c r="S90" s="1"/>
+    </row>
+    <row r="91" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -2234,14 +2476,16 @@
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
       <c r="K91" s="3"/>
-      <c r="L91" s="3"/>
+      <c r="L91" s="9"/>
       <c r="M91" s="3"/>
       <c r="N91" s="3"/>
       <c r="O91" s="3"/>
       <c r="P91" s="3"/>
-      <c r="Q91" s="1"/>
-    </row>
-    <row r="92" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q91" s="3"/>
+      <c r="R91" s="3"/>
+      <c r="S91" s="1"/>
+    </row>
+    <row r="92" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -2253,14 +2497,16 @@
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
       <c r="K92" s="3"/>
-      <c r="L92" s="3"/>
+      <c r="L92" s="9"/>
       <c r="M92" s="3"/>
       <c r="N92" s="3"/>
       <c r="O92" s="3"/>
       <c r="P92" s="3"/>
-      <c r="Q92" s="1"/>
-    </row>
-    <row r="93" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q92" s="3"/>
+      <c r="R92" s="3"/>
+      <c r="S92" s="1"/>
+    </row>
+    <row r="93" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -2272,14 +2518,16 @@
       <c r="I93" s="3"/>
       <c r="J93" s="3"/>
       <c r="K93" s="3"/>
-      <c r="L93" s="3"/>
+      <c r="L93" s="9"/>
       <c r="M93" s="3"/>
       <c r="N93" s="3"/>
       <c r="O93" s="3"/>
       <c r="P93" s="3"/>
-      <c r="Q93" s="1"/>
-    </row>
-    <row r="94" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q93" s="3"/>
+      <c r="R93" s="3"/>
+      <c r="S93" s="1"/>
+    </row>
+    <row r="94" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -2291,14 +2539,16 @@
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
       <c r="K94" s="3"/>
-      <c r="L94" s="3"/>
+      <c r="L94" s="9"/>
       <c r="M94" s="3"/>
       <c r="N94" s="3"/>
       <c r="O94" s="3"/>
       <c r="P94" s="3"/>
-      <c r="Q94" s="1"/>
-    </row>
-    <row r="95" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q94" s="3"/>
+      <c r="R94" s="3"/>
+      <c r="S94" s="1"/>
+    </row>
+    <row r="95" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -2310,14 +2560,16 @@
       <c r="I95" s="3"/>
       <c r="J95" s="3"/>
       <c r="K95" s="3"/>
-      <c r="L95" s="3"/>
+      <c r="L95" s="9"/>
       <c r="M95" s="3"/>
       <c r="N95" s="3"/>
       <c r="O95" s="3"/>
       <c r="P95" s="3"/>
-      <c r="Q95" s="1"/>
-    </row>
-    <row r="96" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q95" s="3"/>
+      <c r="R95" s="3"/>
+      <c r="S95" s="1"/>
+    </row>
+    <row r="96" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -2329,14 +2581,16 @@
       <c r="I96" s="3"/>
       <c r="J96" s="3"/>
       <c r="K96" s="3"/>
-      <c r="L96" s="3"/>
+      <c r="L96" s="9"/>
       <c r="M96" s="3"/>
       <c r="N96" s="3"/>
       <c r="O96" s="3"/>
       <c r="P96" s="3"/>
-      <c r="Q96" s="1"/>
-    </row>
-    <row r="97" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q96" s="3"/>
+      <c r="R96" s="3"/>
+      <c r="S96" s="1"/>
+    </row>
+    <row r="97" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -2348,14 +2602,16 @@
       <c r="I97" s="3"/>
       <c r="J97" s="3"/>
       <c r="K97" s="3"/>
-      <c r="L97" s="3"/>
+      <c r="L97" s="9"/>
       <c r="M97" s="3"/>
       <c r="N97" s="3"/>
       <c r="O97" s="3"/>
       <c r="P97" s="3"/>
-      <c r="Q97" s="1"/>
-    </row>
-    <row r="98" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q97" s="3"/>
+      <c r="R97" s="3"/>
+      <c r="S97" s="1"/>
+    </row>
+    <row r="98" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -2367,14 +2623,16 @@
       <c r="I98" s="3"/>
       <c r="J98" s="3"/>
       <c r="K98" s="3"/>
-      <c r="L98" s="3"/>
+      <c r="L98" s="9"/>
       <c r="M98" s="3"/>
       <c r="N98" s="3"/>
       <c r="O98" s="3"/>
       <c r="P98" s="3"/>
-      <c r="Q98" s="1"/>
-    </row>
-    <row r="99" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q98" s="3"/>
+      <c r="R98" s="3"/>
+      <c r="S98" s="1"/>
+    </row>
+    <row r="99" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -2386,14 +2644,16 @@
       <c r="I99" s="3"/>
       <c r="J99" s="3"/>
       <c r="K99" s="3"/>
-      <c r="L99" s="3"/>
+      <c r="L99" s="9"/>
       <c r="M99" s="3"/>
       <c r="N99" s="3"/>
       <c r="O99" s="3"/>
       <c r="P99" s="3"/>
-      <c r="Q99" s="1"/>
-    </row>
-    <row r="100" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q99" s="3"/>
+      <c r="R99" s="3"/>
+      <c r="S99" s="1"/>
+    </row>
+    <row r="100" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -2405,14 +2665,16 @@
       <c r="I100" s="3"/>
       <c r="J100" s="3"/>
       <c r="K100" s="3"/>
-      <c r="L100" s="3"/>
+      <c r="L100" s="9"/>
       <c r="M100" s="3"/>
       <c r="N100" s="3"/>
       <c r="O100" s="3"/>
       <c r="P100" s="3"/>
-      <c r="Q100" s="1"/>
-    </row>
-    <row r="101" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q100" s="3"/>
+      <c r="R100" s="3"/>
+      <c r="S100" s="1"/>
+    </row>
+    <row r="101" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -2424,14 +2686,16 @@
       <c r="I101" s="3"/>
       <c r="J101" s="3"/>
       <c r="K101" s="3"/>
-      <c r="L101" s="3"/>
+      <c r="L101" s="9"/>
       <c r="M101" s="3"/>
       <c r="N101" s="3"/>
       <c r="O101" s="3"/>
       <c r="P101" s="3"/>
-      <c r="Q101" s="1"/>
-    </row>
-    <row r="102" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q101" s="3"/>
+      <c r="R101" s="3"/>
+      <c r="S101" s="1"/>
+    </row>
+    <row r="102" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -2443,14 +2707,16 @@
       <c r="I102" s="3"/>
       <c r="J102" s="3"/>
       <c r="K102" s="3"/>
-      <c r="L102" s="3"/>
+      <c r="L102" s="9"/>
       <c r="M102" s="3"/>
       <c r="N102" s="3"/>
       <c r="O102" s="3"/>
       <c r="P102" s="3"/>
-      <c r="Q102" s="1"/>
-    </row>
-    <row r="103" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q102" s="3"/>
+      <c r="R102" s="3"/>
+      <c r="S102" s="1"/>
+    </row>
+    <row r="103" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -2462,14 +2728,16 @@
       <c r="I103" s="3"/>
       <c r="J103" s="3"/>
       <c r="K103" s="3"/>
-      <c r="L103" s="3"/>
+      <c r="L103" s="9"/>
       <c r="M103" s="3"/>
       <c r="N103" s="3"/>
       <c r="O103" s="3"/>
       <c r="P103" s="3"/>
-      <c r="Q103" s="1"/>
-    </row>
-    <row r="104" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q103" s="3"/>
+      <c r="R103" s="3"/>
+      <c r="S103" s="1"/>
+    </row>
+    <row r="104" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -2481,14 +2749,16 @@
       <c r="I104" s="3"/>
       <c r="J104" s="3"/>
       <c r="K104" s="3"/>
-      <c r="L104" s="3"/>
+      <c r="L104" s="9"/>
       <c r="M104" s="3"/>
       <c r="N104" s="3"/>
       <c r="O104" s="3"/>
       <c r="P104" s="3"/>
-      <c r="Q104" s="1"/>
-    </row>
-    <row r="105" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q104" s="3"/>
+      <c r="R104" s="3"/>
+      <c r="S104" s="1"/>
+    </row>
+    <row r="105" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -2500,14 +2770,16 @@
       <c r="I105" s="3"/>
       <c r="J105" s="3"/>
       <c r="K105" s="3"/>
-      <c r="L105" s="3"/>
+      <c r="L105" s="9"/>
       <c r="M105" s="3"/>
       <c r="N105" s="3"/>
       <c r="O105" s="3"/>
       <c r="P105" s="3"/>
-      <c r="Q105" s="1"/>
-    </row>
-    <row r="106" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q105" s="3"/>
+      <c r="R105" s="3"/>
+      <c r="S105" s="1"/>
+    </row>
+    <row r="106" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -2519,14 +2791,16 @@
       <c r="I106" s="3"/>
       <c r="J106" s="3"/>
       <c r="K106" s="3"/>
-      <c r="L106" s="3"/>
+      <c r="L106" s="9"/>
       <c r="M106" s="3"/>
       <c r="N106" s="3"/>
       <c r="O106" s="3"/>
       <c r="P106" s="3"/>
-      <c r="Q106" s="1"/>
-    </row>
-    <row r="107" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q106" s="3"/>
+      <c r="R106" s="3"/>
+      <c r="S106" s="1"/>
+    </row>
+    <row r="107" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -2538,14 +2812,16 @@
       <c r="I107" s="3"/>
       <c r="J107" s="3"/>
       <c r="K107" s="3"/>
-      <c r="L107" s="3"/>
+      <c r="L107" s="9"/>
       <c r="M107" s="3"/>
       <c r="N107" s="3"/>
       <c r="O107" s="3"/>
       <c r="P107" s="3"/>
-      <c r="Q107" s="1"/>
-    </row>
-    <row r="108" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q107" s="3"/>
+      <c r="R107" s="3"/>
+      <c r="S107" s="1"/>
+    </row>
+    <row r="108" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -2557,14 +2833,16 @@
       <c r="I108" s="3"/>
       <c r="J108" s="3"/>
       <c r="K108" s="3"/>
-      <c r="L108" s="3"/>
+      <c r="L108" s="9"/>
       <c r="M108" s="3"/>
       <c r="N108" s="3"/>
       <c r="O108" s="3"/>
       <c r="P108" s="3"/>
-      <c r="Q108" s="1"/>
-    </row>
-    <row r="109" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q108" s="3"/>
+      <c r="R108" s="3"/>
+      <c r="S108" s="1"/>
+    </row>
+    <row r="109" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -2576,14 +2854,16 @@
       <c r="I109" s="3"/>
       <c r="J109" s="3"/>
       <c r="K109" s="3"/>
-      <c r="L109" s="3"/>
+      <c r="L109" s="9"/>
       <c r="M109" s="3"/>
       <c r="N109" s="3"/>
       <c r="O109" s="3"/>
       <c r="P109" s="3"/>
-      <c r="Q109" s="1"/>
-    </row>
-    <row r="110" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q109" s="3"/>
+      <c r="R109" s="3"/>
+      <c r="S109" s="1"/>
+    </row>
+    <row r="110" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -2595,14 +2875,16 @@
       <c r="I110" s="3"/>
       <c r="J110" s="3"/>
       <c r="K110" s="3"/>
-      <c r="L110" s="3"/>
+      <c r="L110" s="9"/>
       <c r="M110" s="3"/>
       <c r="N110" s="3"/>
       <c r="O110" s="3"/>
       <c r="P110" s="3"/>
-      <c r="Q110" s="1"/>
-    </row>
-    <row r="111" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q110" s="3"/>
+      <c r="R110" s="3"/>
+      <c r="S110" s="1"/>
+    </row>
+    <row r="111" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -2614,14 +2896,16 @@
       <c r="I111" s="3"/>
       <c r="J111" s="3"/>
       <c r="K111" s="3"/>
-      <c r="L111" s="3"/>
+      <c r="L111" s="9"/>
       <c r="M111" s="3"/>
       <c r="N111" s="3"/>
       <c r="O111" s="3"/>
       <c r="P111" s="3"/>
-      <c r="Q111" s="1"/>
-    </row>
-    <row r="112" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q111" s="3"/>
+      <c r="R111" s="3"/>
+      <c r="S111" s="1"/>
+    </row>
+    <row r="112" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -2633,14 +2917,16 @@
       <c r="I112" s="3"/>
       <c r="J112" s="3"/>
       <c r="K112" s="3"/>
-      <c r="L112" s="3"/>
+      <c r="L112" s="9"/>
       <c r="M112" s="3"/>
       <c r="N112" s="3"/>
       <c r="O112" s="3"/>
       <c r="P112" s="3"/>
-      <c r="Q112" s="1"/>
-    </row>
-    <row r="113" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q112" s="3"/>
+      <c r="R112" s="3"/>
+      <c r="S112" s="1"/>
+    </row>
+    <row r="113" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -2652,14 +2938,16 @@
       <c r="I113" s="3"/>
       <c r="J113" s="3"/>
       <c r="K113" s="3"/>
-      <c r="L113" s="3"/>
+      <c r="L113" s="9"/>
       <c r="M113" s="3"/>
       <c r="N113" s="3"/>
       <c r="O113" s="3"/>
       <c r="P113" s="3"/>
-      <c r="Q113" s="1"/>
-    </row>
-    <row r="114" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q113" s="3"/>
+      <c r="R113" s="3"/>
+      <c r="S113" s="1"/>
+    </row>
+    <row r="114" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -2671,14 +2959,16 @@
       <c r="I114" s="3"/>
       <c r="J114" s="3"/>
       <c r="K114" s="3"/>
-      <c r="L114" s="3"/>
+      <c r="L114" s="9"/>
       <c r="M114" s="3"/>
       <c r="N114" s="3"/>
       <c r="O114" s="3"/>
       <c r="P114" s="3"/>
-      <c r="Q114" s="1"/>
-    </row>
-    <row r="115" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q114" s="3"/>
+      <c r="R114" s="3"/>
+      <c r="S114" s="1"/>
+    </row>
+    <row r="115" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -2690,14 +2980,16 @@
       <c r="I115" s="3"/>
       <c r="J115" s="3"/>
       <c r="K115" s="3"/>
-      <c r="L115" s="3"/>
+      <c r="L115" s="9"/>
       <c r="M115" s="3"/>
       <c r="N115" s="3"/>
       <c r="O115" s="3"/>
       <c r="P115" s="3"/>
-      <c r="Q115" s="1"/>
-    </row>
-    <row r="116" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q115" s="3"/>
+      <c r="R115" s="3"/>
+      <c r="S115" s="1"/>
+    </row>
+    <row r="116" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -2709,14 +3001,16 @@
       <c r="I116" s="3"/>
       <c r="J116" s="3"/>
       <c r="K116" s="3"/>
-      <c r="L116" s="3"/>
+      <c r="L116" s="9"/>
       <c r="M116" s="3"/>
       <c r="N116" s="3"/>
       <c r="O116" s="3"/>
       <c r="P116" s="3"/>
-      <c r="Q116" s="1"/>
-    </row>
-    <row r="117" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q116" s="3"/>
+      <c r="R116" s="3"/>
+      <c r="S116" s="1"/>
+    </row>
+    <row r="117" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -2728,14 +3022,16 @@
       <c r="I117" s="3"/>
       <c r="J117" s="3"/>
       <c r="K117" s="3"/>
-      <c r="L117" s="3"/>
+      <c r="L117" s="9"/>
       <c r="M117" s="3"/>
       <c r="N117" s="3"/>
       <c r="O117" s="3"/>
       <c r="P117" s="3"/>
-      <c r="Q117" s="1"/>
-    </row>
-    <row r="118" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q117" s="3"/>
+      <c r="R117" s="3"/>
+      <c r="S117" s="1"/>
+    </row>
+    <row r="118" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -2747,14 +3043,16 @@
       <c r="I118" s="3"/>
       <c r="J118" s="3"/>
       <c r="K118" s="3"/>
-      <c r="L118" s="3"/>
+      <c r="L118" s="9"/>
       <c r="M118" s="3"/>
       <c r="N118" s="3"/>
       <c r="O118" s="3"/>
       <c r="P118" s="3"/>
-      <c r="Q118" s="1"/>
-    </row>
-    <row r="119" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q118" s="3"/>
+      <c r="R118" s="3"/>
+      <c r="S118" s="1"/>
+    </row>
+    <row r="119" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -2766,14 +3064,16 @@
       <c r="I119" s="3"/>
       <c r="J119" s="3"/>
       <c r="K119" s="3"/>
-      <c r="L119" s="3"/>
+      <c r="L119" s="9"/>
       <c r="M119" s="3"/>
       <c r="N119" s="3"/>
       <c r="O119" s="3"/>
       <c r="P119" s="3"/>
-      <c r="Q119" s="1"/>
-    </row>
-    <row r="120" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q119" s="3"/>
+      <c r="R119" s="3"/>
+      <c r="S119" s="1"/>
+    </row>
+    <row r="120" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -2785,14 +3085,16 @@
       <c r="I120" s="3"/>
       <c r="J120" s="3"/>
       <c r="K120" s="3"/>
-      <c r="L120" s="3"/>
+      <c r="L120" s="9"/>
       <c r="M120" s="3"/>
       <c r="N120" s="3"/>
       <c r="O120" s="3"/>
       <c r="P120" s="3"/>
-      <c r="Q120" s="1"/>
-    </row>
-    <row r="121" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q120" s="3"/>
+      <c r="R120" s="3"/>
+      <c r="S120" s="1"/>
+    </row>
+    <row r="121" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -2804,14 +3106,16 @@
       <c r="I121" s="3"/>
       <c r="J121" s="3"/>
       <c r="K121" s="3"/>
-      <c r="L121" s="3"/>
+      <c r="L121" s="9"/>
       <c r="M121" s="3"/>
       <c r="N121" s="3"/>
       <c r="O121" s="3"/>
       <c r="P121" s="3"/>
-      <c r="Q121" s="1"/>
-    </row>
-    <row r="122" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q121" s="3"/>
+      <c r="R121" s="3"/>
+      <c r="S121" s="1"/>
+    </row>
+    <row r="122" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -2823,14 +3127,16 @@
       <c r="I122" s="3"/>
       <c r="J122" s="3"/>
       <c r="K122" s="3"/>
-      <c r="L122" s="3"/>
+      <c r="L122" s="9"/>
       <c r="M122" s="3"/>
       <c r="N122" s="3"/>
       <c r="O122" s="3"/>
       <c r="P122" s="3"/>
-      <c r="Q122" s="1"/>
-    </row>
-    <row r="123" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q122" s="3"/>
+      <c r="R122" s="3"/>
+      <c r="S122" s="1"/>
+    </row>
+    <row r="123" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -2842,14 +3148,16 @@
       <c r="I123" s="3"/>
       <c r="J123" s="3"/>
       <c r="K123" s="3"/>
-      <c r="L123" s="3"/>
+      <c r="L123" s="9"/>
       <c r="M123" s="3"/>
       <c r="N123" s="3"/>
       <c r="O123" s="3"/>
       <c r="P123" s="3"/>
-      <c r="Q123" s="1"/>
-    </row>
-    <row r="124" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q123" s="3"/>
+      <c r="R123" s="3"/>
+      <c r="S123" s="1"/>
+    </row>
+    <row r="124" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -2861,14 +3169,16 @@
       <c r="I124" s="3"/>
       <c r="J124" s="3"/>
       <c r="K124" s="3"/>
-      <c r="L124" s="3"/>
+      <c r="L124" s="9"/>
       <c r="M124" s="3"/>
       <c r="N124" s="3"/>
       <c r="O124" s="3"/>
       <c r="P124" s="3"/>
-      <c r="Q124" s="1"/>
-    </row>
-    <row r="125" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q124" s="3"/>
+      <c r="R124" s="3"/>
+      <c r="S124" s="1"/>
+    </row>
+    <row r="125" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -2880,14 +3190,16 @@
       <c r="I125" s="3"/>
       <c r="J125" s="3"/>
       <c r="K125" s="3"/>
-      <c r="L125" s="3"/>
+      <c r="L125" s="9"/>
       <c r="M125" s="3"/>
       <c r="N125" s="3"/>
       <c r="O125" s="3"/>
       <c r="P125" s="3"/>
-      <c r="Q125" s="1"/>
-    </row>
-    <row r="126" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q125" s="3"/>
+      <c r="R125" s="3"/>
+      <c r="S125" s="1"/>
+    </row>
+    <row r="126" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -2899,14 +3211,16 @@
       <c r="I126" s="3"/>
       <c r="J126" s="3"/>
       <c r="K126" s="3"/>
-      <c r="L126" s="3"/>
+      <c r="L126" s="9"/>
       <c r="M126" s="3"/>
       <c r="N126" s="3"/>
       <c r="O126" s="3"/>
       <c r="P126" s="3"/>
-      <c r="Q126" s="1"/>
-    </row>
-    <row r="127" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q126" s="3"/>
+      <c r="R126" s="3"/>
+      <c r="S126" s="1"/>
+    </row>
+    <row r="127" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -2918,14 +3232,16 @@
       <c r="I127" s="3"/>
       <c r="J127" s="3"/>
       <c r="K127" s="3"/>
-      <c r="L127" s="3"/>
+      <c r="L127" s="9"/>
       <c r="M127" s="3"/>
       <c r="N127" s="3"/>
       <c r="O127" s="3"/>
       <c r="P127" s="3"/>
-      <c r="Q127" s="1"/>
-    </row>
-    <row r="128" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q127" s="3"/>
+      <c r="R127" s="3"/>
+      <c r="S127" s="1"/>
+    </row>
+    <row r="128" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -2937,14 +3253,16 @@
       <c r="I128" s="3"/>
       <c r="J128" s="3"/>
       <c r="K128" s="3"/>
-      <c r="L128" s="3"/>
+      <c r="L128" s="9"/>
       <c r="M128" s="3"/>
       <c r="N128" s="3"/>
       <c r="O128" s="3"/>
       <c r="P128" s="3"/>
-      <c r="Q128" s="1"/>
-    </row>
-    <row r="129" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q128" s="3"/>
+      <c r="R128" s="3"/>
+      <c r="S128" s="1"/>
+    </row>
+    <row r="129" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -2956,14 +3274,16 @@
       <c r="I129" s="3"/>
       <c r="J129" s="3"/>
       <c r="K129" s="3"/>
-      <c r="L129" s="3"/>
+      <c r="L129" s="9"/>
       <c r="M129" s="3"/>
       <c r="N129" s="3"/>
       <c r="O129" s="3"/>
       <c r="P129" s="3"/>
-      <c r="Q129" s="1"/>
-    </row>
-    <row r="130" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q129" s="3"/>
+      <c r="R129" s="3"/>
+      <c r="S129" s="1"/>
+    </row>
+    <row r="130" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A130" s="1"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -2975,14 +3295,16 @@
       <c r="I130" s="3"/>
       <c r="J130" s="3"/>
       <c r="K130" s="3"/>
-      <c r="L130" s="3"/>
+      <c r="L130" s="9"/>
       <c r="M130" s="3"/>
       <c r="N130" s="3"/>
       <c r="O130" s="3"/>
       <c r="P130" s="3"/>
-      <c r="Q130" s="1"/>
-    </row>
-    <row r="131" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q130" s="3"/>
+      <c r="R130" s="3"/>
+      <c r="S130" s="1"/>
+    </row>
+    <row r="131" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A131" s="1"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -2994,14 +3316,16 @@
       <c r="I131" s="3"/>
       <c r="J131" s="3"/>
       <c r="K131" s="3"/>
-      <c r="L131" s="3"/>
+      <c r="L131" s="9"/>
       <c r="M131" s="3"/>
       <c r="N131" s="3"/>
       <c r="O131" s="3"/>
       <c r="P131" s="3"/>
-      <c r="Q131" s="1"/>
-    </row>
-    <row r="132" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q131" s="3"/>
+      <c r="R131" s="3"/>
+      <c r="S131" s="1"/>
+    </row>
+    <row r="132" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -3013,14 +3337,16 @@
       <c r="I132" s="3"/>
       <c r="J132" s="3"/>
       <c r="K132" s="3"/>
-      <c r="L132" s="3"/>
+      <c r="L132" s="9"/>
       <c r="M132" s="3"/>
       <c r="N132" s="3"/>
       <c r="O132" s="3"/>
       <c r="P132" s="3"/>
-      <c r="Q132" s="1"/>
-    </row>
-    <row r="133" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q132" s="3"/>
+      <c r="R132" s="3"/>
+      <c r="S132" s="1"/>
+    </row>
+    <row r="133" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>
@@ -3032,14 +3358,16 @@
       <c r="I133" s="3"/>
       <c r="J133" s="3"/>
       <c r="K133" s="3"/>
-      <c r="L133" s="3"/>
+      <c r="L133" s="9"/>
       <c r="M133" s="3"/>
       <c r="N133" s="3"/>
       <c r="O133" s="3"/>
       <c r="P133" s="3"/>
-      <c r="Q133" s="1"/>
-    </row>
-    <row r="134" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q133" s="3"/>
+      <c r="R133" s="3"/>
+      <c r="S133" s="1"/>
+    </row>
+    <row r="134" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="3"/>
       <c r="C134" s="3"/>
@@ -3051,14 +3379,16 @@
       <c r="I134" s="3"/>
       <c r="J134" s="3"/>
       <c r="K134" s="3"/>
-      <c r="L134" s="3"/>
+      <c r="L134" s="9"/>
       <c r="M134" s="3"/>
       <c r="N134" s="3"/>
       <c r="O134" s="3"/>
       <c r="P134" s="3"/>
-      <c r="Q134" s="1"/>
-    </row>
-    <row r="135" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q134" s="3"/>
+      <c r="R134" s="3"/>
+      <c r="S134" s="1"/>
+    </row>
+    <row r="135" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -3070,14 +3400,16 @@
       <c r="I135" s="3"/>
       <c r="J135" s="3"/>
       <c r="K135" s="3"/>
-      <c r="L135" s="3"/>
+      <c r="L135" s="9"/>
       <c r="M135" s="3"/>
       <c r="N135" s="3"/>
       <c r="O135" s="3"/>
       <c r="P135" s="3"/>
-      <c r="Q135" s="1"/>
-    </row>
-    <row r="136" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q135" s="3"/>
+      <c r="R135" s="3"/>
+      <c r="S135" s="1"/>
+    </row>
+    <row r="136" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
@@ -3089,14 +3421,16 @@
       <c r="I136" s="3"/>
       <c r="J136" s="3"/>
       <c r="K136" s="3"/>
-      <c r="L136" s="3"/>
+      <c r="L136" s="9"/>
       <c r="M136" s="3"/>
       <c r="N136" s="3"/>
       <c r="O136" s="3"/>
       <c r="P136" s="3"/>
-      <c r="Q136" s="1"/>
-    </row>
-    <row r="137" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q136" s="3"/>
+      <c r="R136" s="3"/>
+      <c r="S136" s="1"/>
+    </row>
+    <row r="137" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A137" s="1"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
@@ -3108,14 +3442,16 @@
       <c r="I137" s="3"/>
       <c r="J137" s="3"/>
       <c r="K137" s="3"/>
-      <c r="L137" s="3"/>
+      <c r="L137" s="9"/>
       <c r="M137" s="3"/>
       <c r="N137" s="3"/>
       <c r="O137" s="3"/>
       <c r="P137" s="3"/>
-      <c r="Q137" s="1"/>
-    </row>
-    <row r="138" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q137" s="3"/>
+      <c r="R137" s="3"/>
+      <c r="S137" s="1"/>
+    </row>
+    <row r="138" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A138" s="1"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
@@ -3127,14 +3463,16 @@
       <c r="I138" s="3"/>
       <c r="J138" s="3"/>
       <c r="K138" s="3"/>
-      <c r="L138" s="3"/>
+      <c r="L138" s="9"/>
       <c r="M138" s="3"/>
       <c r="N138" s="3"/>
       <c r="O138" s="3"/>
       <c r="P138" s="3"/>
-      <c r="Q138" s="1"/>
-    </row>
-    <row r="139" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q138" s="3"/>
+      <c r="R138" s="3"/>
+      <c r="S138" s="1"/>
+    </row>
+    <row r="139" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A139" s="1"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
@@ -3146,14 +3484,16 @@
       <c r="I139" s="3"/>
       <c r="J139" s="3"/>
       <c r="K139" s="3"/>
-      <c r="L139" s="3"/>
+      <c r="L139" s="9"/>
       <c r="M139" s="3"/>
       <c r="N139" s="3"/>
       <c r="O139" s="3"/>
       <c r="P139" s="3"/>
-      <c r="Q139" s="1"/>
-    </row>
-    <row r="140" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q139" s="3"/>
+      <c r="R139" s="3"/>
+      <c r="S139" s="1"/>
+    </row>
+    <row r="140" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A140" s="1"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
@@ -3165,14 +3505,16 @@
       <c r="I140" s="3"/>
       <c r="J140" s="3"/>
       <c r="K140" s="3"/>
-      <c r="L140" s="3"/>
+      <c r="L140" s="9"/>
       <c r="M140" s="3"/>
       <c r="N140" s="3"/>
       <c r="O140" s="3"/>
       <c r="P140" s="3"/>
-      <c r="Q140" s="1"/>
-    </row>
-    <row r="141" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q140" s="3"/>
+      <c r="R140" s="3"/>
+      <c r="S140" s="1"/>
+    </row>
+    <row r="141" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A141" s="1"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
@@ -3184,14 +3526,16 @@
       <c r="I141" s="3"/>
       <c r="J141" s="3"/>
       <c r="K141" s="3"/>
-      <c r="L141" s="3"/>
+      <c r="L141" s="9"/>
       <c r="M141" s="3"/>
       <c r="N141" s="3"/>
       <c r="O141" s="3"/>
       <c r="P141" s="3"/>
-      <c r="Q141" s="1"/>
-    </row>
-    <row r="142" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q141" s="3"/>
+      <c r="R141" s="3"/>
+      <c r="S141" s="1"/>
+    </row>
+    <row r="142" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A142" s="1"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
@@ -3203,14 +3547,16 @@
       <c r="I142" s="3"/>
       <c r="J142" s="3"/>
       <c r="K142" s="3"/>
-      <c r="L142" s="3"/>
+      <c r="L142" s="9"/>
       <c r="M142" s="3"/>
       <c r="N142" s="3"/>
       <c r="O142" s="3"/>
       <c r="P142" s="3"/>
-      <c r="Q142" s="1"/>
-    </row>
-    <row r="143" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q142" s="3"/>
+      <c r="R142" s="3"/>
+      <c r="S142" s="1"/>
+    </row>
+    <row r="143" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A143" s="1"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
@@ -3222,14 +3568,16 @@
       <c r="I143" s="3"/>
       <c r="J143" s="3"/>
       <c r="K143" s="3"/>
-      <c r="L143" s="3"/>
+      <c r="L143" s="9"/>
       <c r="M143" s="3"/>
       <c r="N143" s="3"/>
       <c r="O143" s="3"/>
       <c r="P143" s="3"/>
-      <c r="Q143" s="1"/>
-    </row>
-    <row r="144" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q143" s="3"/>
+      <c r="R143" s="3"/>
+      <c r="S143" s="1"/>
+    </row>
+    <row r="144" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A144" s="1"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
@@ -3241,14 +3589,16 @@
       <c r="I144" s="3"/>
       <c r="J144" s="3"/>
       <c r="K144" s="3"/>
-      <c r="L144" s="3"/>
+      <c r="L144" s="9"/>
       <c r="M144" s="3"/>
       <c r="N144" s="3"/>
       <c r="O144" s="3"/>
       <c r="P144" s="3"/>
-      <c r="Q144" s="1"/>
-    </row>
-    <row r="145" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q144" s="3"/>
+      <c r="R144" s="3"/>
+      <c r="S144" s="1"/>
+    </row>
+    <row r="145" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
@@ -3260,14 +3610,16 @@
       <c r="I145" s="3"/>
       <c r="J145" s="3"/>
       <c r="K145" s="3"/>
-      <c r="L145" s="3"/>
+      <c r="L145" s="9"/>
       <c r="M145" s="3"/>
       <c r="N145" s="3"/>
       <c r="O145" s="3"/>
       <c r="P145" s="3"/>
-      <c r="Q145" s="1"/>
-    </row>
-    <row r="146" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q145" s="3"/>
+      <c r="R145" s="3"/>
+      <c r="S145" s="1"/>
+    </row>
+    <row r="146" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A146" s="1"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
@@ -3279,14 +3631,16 @@
       <c r="I146" s="3"/>
       <c r="J146" s="3"/>
       <c r="K146" s="3"/>
-      <c r="L146" s="3"/>
+      <c r="L146" s="9"/>
       <c r="M146" s="3"/>
       <c r="N146" s="3"/>
       <c r="O146" s="3"/>
       <c r="P146" s="3"/>
-      <c r="Q146" s="1"/>
-    </row>
-    <row r="147" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q146" s="3"/>
+      <c r="R146" s="3"/>
+      <c r="S146" s="1"/>
+    </row>
+    <row r="147" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A147" s="1"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
@@ -3298,14 +3652,16 @@
       <c r="I147" s="3"/>
       <c r="J147" s="3"/>
       <c r="K147" s="3"/>
-      <c r="L147" s="3"/>
+      <c r="L147" s="9"/>
       <c r="M147" s="3"/>
       <c r="N147" s="3"/>
       <c r="O147" s="3"/>
       <c r="P147" s="3"/>
-      <c r="Q147" s="1"/>
-    </row>
-    <row r="148" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q147" s="3"/>
+      <c r="R147" s="3"/>
+      <c r="S147" s="1"/>
+    </row>
+    <row r="148" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A148" s="1"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
@@ -3317,14 +3673,16 @@
       <c r="I148" s="3"/>
       <c r="J148" s="3"/>
       <c r="K148" s="3"/>
-      <c r="L148" s="3"/>
+      <c r="L148" s="9"/>
       <c r="M148" s="3"/>
       <c r="N148" s="3"/>
       <c r="O148" s="3"/>
       <c r="P148" s="3"/>
-      <c r="Q148" s="1"/>
-    </row>
-    <row r="149" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q148" s="3"/>
+      <c r="R148" s="3"/>
+      <c r="S148" s="1"/>
+    </row>
+    <row r="149" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A149" s="1"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
@@ -3336,14 +3694,16 @@
       <c r="I149" s="3"/>
       <c r="J149" s="3"/>
       <c r="K149" s="3"/>
-      <c r="L149" s="3"/>
+      <c r="L149" s="9"/>
       <c r="M149" s="3"/>
       <c r="N149" s="3"/>
       <c r="O149" s="3"/>
       <c r="P149" s="3"/>
-      <c r="Q149" s="1"/>
-    </row>
-    <row r="150" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q149" s="3"/>
+      <c r="R149" s="3"/>
+      <c r="S149" s="1"/>
+    </row>
+    <row r="150" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A150" s="1"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
@@ -3355,14 +3715,16 @@
       <c r="I150" s="3"/>
       <c r="J150" s="3"/>
       <c r="K150" s="3"/>
-      <c r="L150" s="3"/>
+      <c r="L150" s="9"/>
       <c r="M150" s="3"/>
       <c r="N150" s="3"/>
       <c r="O150" s="3"/>
       <c r="P150" s="3"/>
-      <c r="Q150" s="1"/>
-    </row>
-    <row r="151" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q150" s="3"/>
+      <c r="R150" s="3"/>
+      <c r="S150" s="1"/>
+    </row>
+    <row r="151" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A151" s="1"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
@@ -3374,14 +3736,16 @@
       <c r="I151" s="3"/>
       <c r="J151" s="3"/>
       <c r="K151" s="3"/>
-      <c r="L151" s="3"/>
+      <c r="L151" s="9"/>
       <c r="M151" s="3"/>
       <c r="N151" s="3"/>
       <c r="O151" s="3"/>
       <c r="P151" s="3"/>
-      <c r="Q151" s="1"/>
-    </row>
-    <row r="152" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q151" s="3"/>
+      <c r="R151" s="3"/>
+      <c r="S151" s="1"/>
+    </row>
+    <row r="152" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A152" s="1"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
@@ -3393,14 +3757,16 @@
       <c r="I152" s="3"/>
       <c r="J152" s="3"/>
       <c r="K152" s="3"/>
-      <c r="L152" s="3"/>
+      <c r="L152" s="9"/>
       <c r="M152" s="3"/>
       <c r="N152" s="3"/>
       <c r="O152" s="3"/>
       <c r="P152" s="3"/>
-      <c r="Q152" s="1"/>
-    </row>
-    <row r="153" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q152" s="3"/>
+      <c r="R152" s="3"/>
+      <c r="S152" s="1"/>
+    </row>
+    <row r="153" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A153" s="1"/>
       <c r="B153" s="3"/>
       <c r="C153" s="3"/>
@@ -3412,14 +3778,16 @@
       <c r="I153" s="3"/>
       <c r="J153" s="3"/>
       <c r="K153" s="3"/>
-      <c r="L153" s="3"/>
+      <c r="L153" s="9"/>
       <c r="M153" s="3"/>
       <c r="N153" s="3"/>
       <c r="O153" s="3"/>
       <c r="P153" s="3"/>
-      <c r="Q153" s="1"/>
-    </row>
-    <row r="154" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q153" s="3"/>
+      <c r="R153" s="3"/>
+      <c r="S153" s="1"/>
+    </row>
+    <row r="154" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A154" s="1"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
@@ -3431,14 +3799,16 @@
       <c r="I154" s="3"/>
       <c r="J154" s="3"/>
       <c r="K154" s="3"/>
-      <c r="L154" s="3"/>
+      <c r="L154" s="9"/>
       <c r="M154" s="3"/>
       <c r="N154" s="3"/>
       <c r="O154" s="3"/>
       <c r="P154" s="3"/>
-      <c r="Q154" s="1"/>
-    </row>
-    <row r="155" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q154" s="3"/>
+      <c r="R154" s="3"/>
+      <c r="S154" s="1"/>
+    </row>
+    <row r="155" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A155" s="1"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
@@ -3450,14 +3820,16 @@
       <c r="I155" s="3"/>
       <c r="J155" s="3"/>
       <c r="K155" s="3"/>
-      <c r="L155" s="3"/>
+      <c r="L155" s="9"/>
       <c r="M155" s="3"/>
       <c r="N155" s="3"/>
       <c r="O155" s="3"/>
       <c r="P155" s="3"/>
-      <c r="Q155" s="1"/>
-    </row>
-    <row r="156" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q155" s="3"/>
+      <c r="R155" s="3"/>
+      <c r="S155" s="1"/>
+    </row>
+    <row r="156" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A156" s="1"/>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
@@ -3469,14 +3841,16 @@
       <c r="I156" s="3"/>
       <c r="J156" s="3"/>
       <c r="K156" s="3"/>
-      <c r="L156" s="3"/>
+      <c r="L156" s="9"/>
       <c r="M156" s="3"/>
       <c r="N156" s="3"/>
       <c r="O156" s="3"/>
       <c r="P156" s="3"/>
-      <c r="Q156" s="1"/>
-    </row>
-    <row r="157" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q156" s="3"/>
+      <c r="R156" s="3"/>
+      <c r="S156" s="1"/>
+    </row>
+    <row r="157" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A157" s="1"/>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
@@ -3488,14 +3862,16 @@
       <c r="I157" s="3"/>
       <c r="J157" s="3"/>
       <c r="K157" s="3"/>
-      <c r="L157" s="3"/>
+      <c r="L157" s="9"/>
       <c r="M157" s="3"/>
       <c r="N157" s="3"/>
       <c r="O157" s="3"/>
       <c r="P157" s="3"/>
-      <c r="Q157" s="1"/>
-    </row>
-    <row r="158" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q157" s="3"/>
+      <c r="R157" s="3"/>
+      <c r="S157" s="1"/>
+    </row>
+    <row r="158" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A158" s="1"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
@@ -3507,14 +3883,16 @@
       <c r="I158" s="3"/>
       <c r="J158" s="3"/>
       <c r="K158" s="3"/>
-      <c r="L158" s="3"/>
+      <c r="L158" s="9"/>
       <c r="M158" s="3"/>
       <c r="N158" s="3"/>
       <c r="O158" s="3"/>
       <c r="P158" s="3"/>
-      <c r="Q158" s="1"/>
-    </row>
-    <row r="159" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q158" s="3"/>
+      <c r="R158" s="3"/>
+      <c r="S158" s="1"/>
+    </row>
+    <row r="159" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A159" s="1"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
@@ -3526,14 +3904,16 @@
       <c r="I159" s="3"/>
       <c r="J159" s="3"/>
       <c r="K159" s="3"/>
-      <c r="L159" s="3"/>
+      <c r="L159" s="9"/>
       <c r="M159" s="3"/>
       <c r="N159" s="3"/>
       <c r="O159" s="3"/>
       <c r="P159" s="3"/>
-      <c r="Q159" s="1"/>
-    </row>
-    <row r="160" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="Q159" s="3"/>
+      <c r="R159" s="3"/>
+      <c r="S159" s="1"/>
+    </row>
+    <row r="160" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A160" s="1"/>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
@@ -3545,14 +3925,38 @@
       <c r="I160" s="3"/>
       <c r="J160" s="3"/>
       <c r="K160" s="3"/>
-      <c r="L160" s="3"/>
+      <c r="L160" s="9"/>
       <c r="M160" s="3"/>
       <c r="N160" s="3"/>
       <c r="O160" s="3"/>
       <c r="P160" s="3"/>
-      <c r="Q160" s="1"/>
+      <c r="Q160" s="3"/>
+      <c r="R160" s="3"/>
+      <c r="S160" s="1"/>
+    </row>
+    <row r="161" spans="1:19" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="A161" s="1"/>
+      <c r="B161" s="3"/>
+      <c r="C161" s="3"/>
+      <c r="D161" s="3"/>
+      <c r="E161" s="3"/>
+      <c r="F161" s="3"/>
+      <c r="G161" s="3"/>
+      <c r="H161" s="3"/>
+      <c r="I161" s="3"/>
+      <c r="J161" s="3"/>
+      <c r="K161" s="3"/>
+      <c r="L161" s="9"/>
+      <c r="M161" s="3"/>
+      <c r="N161" s="3"/>
+      <c r="O161" s="3"/>
+      <c r="P161" s="3"/>
+      <c r="Q161" s="3"/>
+      <c r="R161" s="3"/>
+      <c r="S161" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: add work as Excel attribute
</commit_message>
<xml_diff>
--- a/frontend/src/components/components/Donor Application Multiple.xlsx
+++ b/frontend/src/components/components/Donor Application Multiple.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\OneDrive - up.edu.ph\Documents\CMSC\2SP\frontend\src\components\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\OneDrive - up.edu.ph\Documents\GitHub\ScholarVision\frontend\src\components\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>Last Name *</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Details *</t>
+  </si>
+  <si>
+    <t>Work</t>
   </si>
 </sst>
 </file>
@@ -495,9 +498,9 @@
   </sheetPr>
   <dimension ref="A1:S161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R2" sqref="R2"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -598,7 +601,9 @@
       <c r="L2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="6"/>
+      <c r="M2" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="N2" s="6" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
fix: final xlsx template
</commit_message>
<xml_diff>
--- a/frontend/src/components/components/Donor Application Multiple.xlsx
+++ b/frontend/src/components/components/Donor Application Multiple.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>Last Name *</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Details *</t>
-  </si>
-  <si>
-    <t>Work</t>
   </si>
 </sst>
 </file>
@@ -601,9 +598,7 @@
       <c r="L2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="M2" s="6"/>
       <c r="N2" s="6" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
fix: list of scholars for specific year
</commit_message>
<xml_diff>
--- a/frontend/src/components/components/Donor Application Multiple.xlsx
+++ b/frontend/src/components/components/Donor Application Multiple.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\OneDrive - up.edu.ph\Documents\GitHub\ScholarVision\frontend\src\components\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\OneDrive - up.edu.ph\Documents\CMSC\2SP\frontend\src\components\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -495,9 +495,9 @@
   </sheetPr>
   <dimension ref="A1:S161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
+      <selection pane="bottomLeft" activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>